<commit_message>
maj compte agents T1 2024 à partir de la PE du T2 24
</commit_message>
<xml_diff>
--- a/Conjoncture - comptes trimestriels/data/smpt.xlsx
+++ b/Conjoncture - comptes trimestriels/data/smpt.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C299"/>
+  <dimension ref="A1:C303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -386,10 +386,10 @@
         <v>17899</v>
       </c>
       <c r="B2">
-        <v>0.8486128517771353</v>
+        <v>0.9119637521776698</v>
       </c>
       <c r="C2">
-        <v>5.18882818549106</v>
+        <v>5.339838170438876</v>
       </c>
     </row>
     <row r="3">
@@ -397,10 +397,10 @@
         <v>17989</v>
       </c>
       <c r="B3">
-        <v>0.8724214197331274</v>
+        <v>0.9400490109972169</v>
       </c>
       <c r="C3">
-        <v>5.225204698056086</v>
+        <v>5.371486739226979</v>
       </c>
     </row>
     <row r="4">
@@ -408,10 +408,10 @@
         <v>18080</v>
       </c>
       <c r="B4">
-        <v>0.8781745007940236</v>
+        <v>0.9456053315760382</v>
       </c>
       <c r="C4">
-        <v>5.379105460262934</v>
+        <v>5.522872624909363</v>
       </c>
     </row>
     <row r="5">
@@ -419,10 +419,10 @@
         <v>18172</v>
       </c>
       <c r="B5">
-        <v>0.8790113741662976</v>
+        <v>0.9432807509623156</v>
       </c>
       <c r="C5">
-        <v>5.404338996761497</v>
+        <v>5.547833345288726</v>
       </c>
     </row>
     <row r="6">
@@ -430,10 +430,10 @@
         <v>18264</v>
       </c>
       <c r="B6">
-        <v>0.9036501440277641</v>
+        <v>0.9691288683785106</v>
       </c>
       <c r="C6">
-        <v>5.481097403417228</v>
+        <v>5.63273450097601</v>
       </c>
     </row>
     <row r="7">
@@ -441,10 +441,10 @@
         <v>18354</v>
       </c>
       <c r="B7">
-        <v>0.9399196759482394</v>
+        <v>1.005772017585642</v>
       </c>
       <c r="C7">
-        <v>5.581494284300094</v>
+        <v>5.737209152810838</v>
       </c>
     </row>
     <row r="8">
@@ -452,10 +452,10 @@
         <v>18445</v>
       </c>
       <c r="B8">
-        <v>0.9753568292029805</v>
+        <v>1.041759491291501</v>
       </c>
       <c r="C8">
-        <v>5.815605754308256</v>
+        <v>5.978329523695642</v>
       </c>
     </row>
     <row r="9">
@@ -463,10 +463,10 @@
         <v>18537</v>
       </c>
       <c r="B9">
-        <v>1.018718710820987</v>
+        <v>1.085864893060459</v>
       </c>
       <c r="C9">
-        <v>5.973754838951565</v>
+        <v>6.151210076920273</v>
       </c>
     </row>
     <row r="10">
@@ -474,10 +474,10 @@
         <v>18629</v>
       </c>
       <c r="B10">
-        <v>1.076978651017729</v>
+        <v>1.146626407350283</v>
       </c>
       <c r="C10">
-        <v>6.278316641471992</v>
+        <v>6.474190518072081</v>
       </c>
     </row>
     <row r="11">
@@ -485,10 +485,10 @@
         <v>18719</v>
       </c>
       <c r="B11">
-        <v>1.166475519695628</v>
+        <v>1.243165693270394</v>
       </c>
       <c r="C11">
-        <v>6.601521156454883</v>
+        <v>6.808039015493986</v>
       </c>
     </row>
     <row r="12">
@@ -496,10 +496,10 @@
         <v>18810</v>
       </c>
       <c r="B12">
-        <v>1.272880019357605</v>
+        <v>1.360148904409423</v>
       </c>
       <c r="C12">
-        <v>6.8452007713945</v>
+        <v>7.061833737853579</v>
       </c>
     </row>
     <row r="13">
@@ -507,10 +507,10 @@
         <v>18902</v>
       </c>
       <c r="B13">
-        <v>1.371819826339079</v>
+        <v>1.468377286283959</v>
       </c>
       <c r="C13">
-        <v>7.193852093483353</v>
+        <v>7.415401838436744</v>
       </c>
     </row>
     <row r="14">
@@ -518,10 +518,10 @@
         <v>18994</v>
       </c>
       <c r="B14">
-        <v>1.430133567604444</v>
+        <v>1.531025622280974</v>
       </c>
       <c r="C14">
-        <v>7.434810925683653</v>
+        <v>7.653546634809047</v>
       </c>
     </row>
     <row r="15">
@@ -529,10 +529,10 @@
         <v>19085</v>
       </c>
       <c r="B15">
-        <v>1.467307585265254</v>
+        <v>1.568919253284763</v>
       </c>
       <c r="C15">
-        <v>7.476762323345125</v>
+        <v>7.695507743818482</v>
       </c>
     </row>
     <row r="16">
@@ -540,10 +540,10 @@
         <v>19176</v>
       </c>
       <c r="B16">
-        <v>1.487265091325445</v>
+        <v>1.587512872624829</v>
       </c>
       <c r="C16">
-        <v>7.507886996517491</v>
+        <v>7.728220747427129</v>
       </c>
     </row>
     <row r="17">
@@ -551,10 +551,10 @@
         <v>19268</v>
       </c>
       <c r="B17">
-        <v>1.497204554737963</v>
+        <v>1.596687811480681</v>
       </c>
       <c r="C17">
-        <v>7.477627920505485</v>
+        <v>7.698086480010718</v>
       </c>
     </row>
     <row r="18">
@@ -562,10 +562,10 @@
         <v>19360</v>
       </c>
       <c r="B18">
-        <v>1.505169125942702</v>
+        <v>1.60526638227522</v>
       </c>
       <c r="C18">
-        <v>7.458418168490763</v>
+        <v>7.676799935311532</v>
       </c>
     </row>
     <row r="19">
@@ -573,10 +573,10 @@
         <v>19450</v>
       </c>
       <c r="B19">
-        <v>1.524674650884924</v>
+        <v>1.625871852635193</v>
       </c>
       <c r="C19">
-        <v>7.451243514936206</v>
+        <v>7.670035969944846</v>
       </c>
     </row>
     <row r="20">
@@ -584,10 +584,10 @@
         <v>19541</v>
       </c>
       <c r="B20">
-        <v>1.540217789696486</v>
+        <v>1.640665235419989</v>
       </c>
       <c r="C20">
-        <v>7.452294034756862</v>
+        <v>7.671338641205576</v>
       </c>
     </row>
     <row r="21">
@@ -595,10 +595,10 @@
         <v>19633</v>
       </c>
       <c r="B21">
-        <v>1.563106905309422</v>
+        <v>1.662908147751186</v>
       </c>
       <c r="C21">
-        <v>7.41518049051058</v>
+        <v>7.635232965054609</v>
       </c>
     </row>
     <row r="22">
@@ -606,10 +606,10 @@
         <v>19725</v>
       </c>
       <c r="B22">
-        <v>1.600426708775696</v>
+        <v>1.700182116399544</v>
       </c>
       <c r="C22">
-        <v>7.478563447277432</v>
+        <v>7.696852517020485</v>
       </c>
     </row>
     <row r="23">
@@ -617,10 +617,10 @@
         <v>19815</v>
       </c>
       <c r="B23">
-        <v>1.638815538141273</v>
+        <v>1.741285128932459</v>
       </c>
       <c r="C23">
-        <v>7.538783355693199</v>
+        <v>7.757518183998162</v>
       </c>
     </row>
     <row r="24">
@@ -628,10 +628,10 @@
         <v>19906</v>
       </c>
       <c r="B24">
-        <v>1.658195248838765</v>
+        <v>1.75980477807504</v>
       </c>
       <c r="C24">
-        <v>7.577616004581508</v>
+        <v>7.796831099351851</v>
       </c>
     </row>
     <row r="25">
@@ -639,10 +639,10 @@
         <v>19998</v>
       </c>
       <c r="B25">
-        <v>1.686683298120805</v>
+        <v>1.790980431718531</v>
       </c>
       <c r="C25">
-        <v>7.601502883913799</v>
+        <v>7.821485273112411</v>
       </c>
     </row>
     <row r="26">
@@ -650,10 +650,10 @@
         <v>20090</v>
       </c>
       <c r="B26">
-        <v>1.717038346509408</v>
+        <v>1.825932353903828</v>
       </c>
       <c r="C26">
-        <v>7.565572360065231</v>
+        <v>7.779996885182437</v>
       </c>
     </row>
     <row r="27">
@@ -661,10 +661,10 @@
         <v>20180</v>
       </c>
       <c r="B27">
-        <v>1.752478245577401</v>
+        <v>1.863577280056423</v>
       </c>
       <c r="C27">
-        <v>7.609176509349805</v>
+        <v>7.824864893790667</v>
       </c>
     </row>
     <row r="28">
@@ -672,10 +672,10 @@
         <v>20271</v>
       </c>
       <c r="B28">
-        <v>1.800816495006601</v>
+        <v>1.910357119673727</v>
       </c>
       <c r="C28">
-        <v>7.652602509562819</v>
+        <v>7.86798043805099</v>
       </c>
     </row>
     <row r="29">
@@ -683,10 +683,10 @@
         <v>20363</v>
       </c>
       <c r="B29">
-        <v>1.853231789176701</v>
+        <v>1.959685823825672</v>
       </c>
       <c r="C29">
-        <v>7.740672190463073</v>
+        <v>7.958808352447906</v>
       </c>
     </row>
     <row r="30">
@@ -694,10 +694,10 @@
         <v>20455</v>
       </c>
       <c r="B30">
-        <v>1.902645501631008</v>
+        <v>2.000815284940289</v>
       </c>
       <c r="C30">
-        <v>7.857373560108076</v>
+        <v>8.085284829046854</v>
       </c>
     </row>
     <row r="31">
@@ -705,10 +705,10 @@
         <v>20546</v>
       </c>
       <c r="B31">
-        <v>1.949314120123532</v>
+        <v>2.045280262429842</v>
       </c>
       <c r="C31">
-        <v>7.94351998035441</v>
+        <v>8.175905087399585</v>
       </c>
     </row>
     <row r="32">
@@ -716,10 +716,10 @@
         <v>20637</v>
       </c>
       <c r="B32">
-        <v>1.993189062038751</v>
+        <v>2.089733517734347</v>
       </c>
       <c r="C32">
-        <v>8.068658760245116</v>
+        <v>8.305136717361712</v>
       </c>
     </row>
     <row r="33">
@@ -727,10 +727,10 @@
         <v>20729</v>
       </c>
       <c r="B33">
-        <v>2.033453253918812</v>
+        <v>2.135157745088329</v>
       </c>
       <c r="C33">
-        <v>8.15174042417056</v>
+        <v>8.390967513549427</v>
       </c>
     </row>
     <row r="34">
@@ -738,10 +738,10 @@
         <v>20821</v>
       </c>
       <c r="B34">
-        <v>2.072334428067237</v>
+        <v>2.184535926044258</v>
       </c>
       <c r="C34">
-        <v>8.1559848395515</v>
+        <v>8.40783821248194</v>
       </c>
     </row>
     <row r="35">
@@ -749,10 +749,10 @@
         <v>20911</v>
       </c>
       <c r="B35">
-        <v>2.121022966490148</v>
+        <v>2.242178137741503</v>
       </c>
       <c r="C35">
-        <v>8.303875150628873</v>
+        <v>8.560040249462283</v>
       </c>
     </row>
     <row r="36">
@@ -760,10 +760,10 @@
         <v>21002</v>
       </c>
       <c r="B36">
-        <v>2.184099996694995</v>
+        <v>2.313392328037552</v>
       </c>
       <c r="C36">
-        <v>8.573184394404857</v>
+        <v>8.828263661171368</v>
       </c>
     </row>
     <row r="37">
@@ -771,10 +771,10 @@
         <v>21094</v>
       </c>
       <c r="B37">
-        <v>2.265468072585544</v>
+        <v>2.402511510766282</v>
       </c>
       <c r="C37">
-        <v>8.884745216851888</v>
+        <v>9.140739167951805</v>
       </c>
     </row>
     <row r="38">
@@ -782,10 +782,10 @@
         <v>21186</v>
       </c>
       <c r="B38">
-        <v>2.35489201084165</v>
+        <v>2.498533240135791</v>
       </c>
       <c r="C38">
-        <v>9.249427777441564</v>
+        <v>9.497770711279232</v>
       </c>
     </row>
     <row r="39">
@@ -793,10 +793,10 @@
         <v>21276</v>
       </c>
       <c r="B39">
-        <v>2.434208166046114</v>
+        <v>2.580415836461362</v>
       </c>
       <c r="C39">
-        <v>9.523317194994364</v>
+        <v>9.779457476502172</v>
       </c>
     </row>
     <row r="40">
@@ -804,10 +804,10 @@
         <v>21367</v>
       </c>
       <c r="B40">
-        <v>2.492294934225937</v>
+        <v>2.636941330712266</v>
       </c>
       <c r="C40">
-        <v>9.636438472572603</v>
+        <v>9.897632531672223</v>
       </c>
     </row>
     <row r="41">
@@ -815,10 +815,10 @@
         <v>21459</v>
       </c>
       <c r="B41">
-        <v>2.538243862871465</v>
+        <v>2.678509734644793</v>
       </c>
       <c r="C41">
-        <v>9.722466406280482</v>
+        <v>9.99203544870913</v>
       </c>
     </row>
     <row r="42">
@@ -826,10 +826,10 @@
         <v>21551</v>
       </c>
       <c r="B42">
-        <v>2.598433323301405</v>
+        <v>2.736051825167075</v>
       </c>
       <c r="C42">
-        <v>9.95905314964229</v>
+        <v>10.24031544243765</v>
       </c>
     </row>
     <row r="43">
@@ -837,10 +837,10 @@
         <v>21641</v>
       </c>
       <c r="B43">
-        <v>2.67098523737608</v>
+        <v>2.810517818126516</v>
       </c>
       <c r="C43">
-        <v>10.05803982349138</v>
+        <v>10.34318576574099</v>
       </c>
     </row>
     <row r="44">
@@ -848,10 +848,10 @@
         <v>21732</v>
       </c>
       <c r="B44">
-        <v>2.727817676092117</v>
+        <v>2.868678454497881</v>
       </c>
       <c r="C44">
-        <v>10.15394319827598</v>
+        <v>10.44462655123891</v>
       </c>
     </row>
     <row r="45">
@@ -859,10 +859,10 @@
         <v>21824</v>
       </c>
       <c r="B45">
-        <v>2.78074265845672</v>
+        <v>2.924709917846087</v>
       </c>
       <c r="C45">
-        <v>10.26771918534334</v>
+        <v>10.55962073439492</v>
       </c>
     </row>
     <row r="46">
@@ -870,10 +870,10 @@
         <v>21916</v>
       </c>
       <c r="B46">
-        <v>2.830324123032142</v>
+        <v>2.981492087875075</v>
       </c>
       <c r="C46">
-        <v>10.33506877431223</v>
+        <v>10.63021602065246</v>
       </c>
     </row>
     <row r="47">
@@ -881,10 +881,10 @@
         <v>22007</v>
       </c>
       <c r="B47">
-        <v>2.884656780301924</v>
+        <v>3.036249966766536</v>
       </c>
       <c r="C47">
-        <v>10.40526475750215</v>
+        <v>10.70197979870404</v>
       </c>
     </row>
     <row r="48">
@@ -892,10 +892,10 @@
         <v>22098</v>
       </c>
       <c r="B48">
-        <v>2.954168526113714</v>
+        <v>3.103311072746574</v>
       </c>
       <c r="C48">
-        <v>10.45950548204476</v>
+        <v>10.76430393269994</v>
       </c>
     </row>
     <row r="49">
@@ -903,10 +903,10 @@
         <v>22190</v>
       </c>
       <c r="B49">
-        <v>3.039594111373707</v>
+        <v>3.181675561146607</v>
       </c>
       <c r="C49">
-        <v>10.51484122522255</v>
+        <v>10.82586775960571</v>
       </c>
     </row>
     <row r="50">
@@ -914,10 +914,10 @@
         <v>22282</v>
       </c>
       <c r="B50">
-        <v>3.117284422996757</v>
+        <v>3.245019838357541</v>
       </c>
       <c r="C50">
-        <v>10.56540606555583</v>
+        <v>10.88295455486391</v>
       </c>
     </row>
     <row r="51">
@@ -925,10 +925,10 @@
         <v>22372</v>
       </c>
       <c r="B51">
-        <v>3.210535229522396</v>
+        <v>3.329202938026841</v>
       </c>
       <c r="C51">
-        <v>10.68602985827363</v>
+        <v>11.00274134062052</v>
       </c>
     </row>
     <row r="52">
@@ -936,10 +936,10 @@
         <v>22463</v>
       </c>
       <c r="B52">
-        <v>3.300776503151447</v>
+        <v>3.411880286337692</v>
       </c>
       <c r="C52">
-        <v>10.77228909525474</v>
+        <v>11.09270660659306</v>
       </c>
     </row>
     <row r="53">
@@ -947,10 +947,10 @@
         <v>22555</v>
       </c>
       <c r="B53">
-        <v>3.393809631341743</v>
+        <v>3.500952865192975</v>
       </c>
       <c r="C53">
-        <v>10.88273395134015</v>
+        <v>11.2008146704091</v>
       </c>
     </row>
     <row r="54">
@@ -958,10 +958,10 @@
         <v>22647</v>
       </c>
       <c r="B54">
-        <v>3.490978979330889</v>
+        <v>3.595331866857863</v>
       </c>
       <c r="C54">
-        <v>11.04504921387833</v>
+        <v>11.36533891780228</v>
       </c>
     </row>
     <row r="55">
@@ -969,10 +969,10 @@
         <v>22737</v>
       </c>
       <c r="B55">
-        <v>3.570989632658998</v>
+        <v>3.674839510970128</v>
       </c>
       <c r="C55">
-        <v>11.16931690265463</v>
+        <v>11.48551117039671</v>
       </c>
     </row>
     <row r="56">
@@ -980,10 +980,10 @@
         <v>22828</v>
       </c>
       <c r="B56">
-        <v>3.652674019449484</v>
+        <v>3.761210113740822</v>
       </c>
       <c r="C56">
-        <v>11.24190523763596</v>
+        <v>11.55569677834987</v>
       </c>
     </row>
     <row r="57">
@@ -991,10 +991,10 @@
         <v>22920</v>
       </c>
       <c r="B57">
-        <v>3.745767661910703</v>
+        <v>3.865866325361232</v>
       </c>
       <c r="C57">
-        <v>11.32162936636525</v>
+        <v>11.6387044186326</v>
       </c>
     </row>
     <row r="58">
@@ -1002,10 +1002,10 @@
         <v>23012</v>
       </c>
       <c r="B58">
-        <v>3.861150808029319</v>
+        <v>3.96558381662054</v>
       </c>
       <c r="C58">
-        <v>11.36324382132478</v>
+        <v>11.69176687269192</v>
       </c>
     </row>
     <row r="59">
@@ -1013,10 +1013,10 @@
         <v>23102</v>
       </c>
       <c r="B59">
-        <v>3.964889827254213</v>
+        <v>4.079254496047796</v>
       </c>
       <c r="C59">
-        <v>11.65885010188</v>
+        <v>11.97413881690756</v>
       </c>
     </row>
     <row r="60">
@@ -1024,10 +1024,10 @@
         <v>23193</v>
       </c>
       <c r="B60">
-        <v>4.06217172118787</v>
+        <v>4.187341039226161</v>
       </c>
       <c r="C60">
-        <v>11.89399448513409</v>
+        <v>12.21220858062742</v>
       </c>
     </row>
     <row r="61">
@@ -1035,10 +1035,10 @@
         <v>23285</v>
       </c>
       <c r="B61">
-        <v>4.158027573182953</v>
+        <v>4.288983328548449</v>
       </c>
       <c r="C61">
-        <v>11.97959219586727</v>
+        <v>12.2997838383475</v>
       </c>
     </row>
     <row r="62">
@@ -1046,10 +1046,10 @@
         <v>23377</v>
       </c>
       <c r="B62">
-        <v>4.247677006068724</v>
+        <v>4.380608302826501</v>
       </c>
       <c r="C62">
-        <v>11.99366530520569</v>
+        <v>12.32625956370368</v>
       </c>
     </row>
     <row r="63">
@@ -1057,10 +1057,10 @@
         <v>23468</v>
       </c>
       <c r="B63">
-        <v>4.337855984043556</v>
+        <v>4.473334877781486</v>
       </c>
       <c r="C63">
-        <v>12.05845053458965</v>
+        <v>12.39480095613668</v>
       </c>
     </row>
     <row r="64">
@@ -1068,10 +1068,10 @@
         <v>23559</v>
       </c>
       <c r="B64">
-        <v>4.414571731526155</v>
+        <v>4.54797557672012</v>
       </c>
       <c r="C64">
-        <v>12.15689450650436</v>
+        <v>12.49159762108912</v>
       </c>
     </row>
     <row r="65">
@@ -1079,10 +1079,10 @@
         <v>23651</v>
       </c>
       <c r="B65">
-        <v>4.50086404071391</v>
+        <v>4.626488439878507</v>
       </c>
       <c r="C65">
-        <v>12.24476622807491</v>
+        <v>12.57572382387303</v>
       </c>
     </row>
     <row r="66">
@@ -1090,10 +1090,10 @@
         <v>23743</v>
       </c>
       <c r="B66">
-        <v>4.574499308208217</v>
+        <v>4.687776804290698</v>
       </c>
       <c r="C66">
-        <v>12.33526975148622</v>
+        <v>12.67598155179204</v>
       </c>
     </row>
     <row r="67">
@@ -1101,10 +1101,10 @@
         <v>23833</v>
       </c>
       <c r="B67">
-        <v>4.653198304244458</v>
+        <v>4.762565294220295</v>
       </c>
       <c r="C67">
-        <v>12.38636748768417</v>
+        <v>12.72937904111179</v>
       </c>
     </row>
     <row r="68">
@@ -1112,10 +1112,10 @@
         <v>23924</v>
       </c>
       <c r="B68">
-        <v>4.725218500259279</v>
+        <v>4.831162070546653</v>
       </c>
       <c r="C68">
-        <v>12.44074756354867</v>
+        <v>12.79133439060583</v>
       </c>
     </row>
     <row r="69">
@@ -1123,10 +1123,10 @@
         <v>24016</v>
       </c>
       <c r="B69">
-        <v>4.799270462007076</v>
+        <v>4.911988625817329</v>
       </c>
       <c r="C69">
-        <v>12.55509486992497</v>
+        <v>12.90654848594362</v>
       </c>
     </row>
     <row r="70">
@@ -1134,10 +1134,10 @@
         <v>24108</v>
       </c>
       <c r="B70">
-        <v>4.865142510594774</v>
+        <v>4.985389117114812</v>
       </c>
       <c r="C70">
-        <v>12.70145809057556</v>
+        <v>13.0456364607463</v>
       </c>
     </row>
     <row r="71">
@@ -1145,10 +1145,10 @@
         <v>24198</v>
       </c>
       <c r="B71">
-        <v>4.941618493055852</v>
+        <v>5.063735834343045</v>
       </c>
       <c r="C71">
-        <v>12.743175911081</v>
+        <v>13.09430433839239</v>
       </c>
     </row>
     <row r="72">
@@ -1156,10 +1156,10 @@
         <v>24289</v>
       </c>
       <c r="B72">
-        <v>5.020682708510872</v>
+        <v>5.14151009272969</v>
       </c>
       <c r="C72">
-        <v>12.84264561721161</v>
+        <v>13.20061162549781</v>
       </c>
     </row>
     <row r="73">
@@ -1167,10 +1167,10 @@
         <v>24381</v>
       </c>
       <c r="B73">
-        <v>5.114968209752521</v>
+        <v>5.232477320505973</v>
       </c>
       <c r="C73">
-        <v>12.91538728159733</v>
+        <v>13.27998266170084</v>
       </c>
     </row>
     <row r="74">
@@ -1178,10 +1178,10 @@
         <v>24473</v>
       </c>
       <c r="B74">
-        <v>5.22712717204477</v>
+        <v>5.334799791369474</v>
       </c>
       <c r="C74">
-        <v>13.04967025242922</v>
+        <v>13.419237118664</v>
       </c>
     </row>
     <row r="75">
@@ -1189,10 +1189,10 @@
         <v>24563</v>
       </c>
       <c r="B75">
-        <v>5.30122110721027</v>
+        <v>5.39868513267513</v>
       </c>
       <c r="C75">
-        <v>13.13310718069467</v>
+        <v>13.51005633364187</v>
       </c>
     </row>
     <row r="76">
@@ -1200,10 +1200,10 @@
         <v>24654</v>
       </c>
       <c r="B76">
-        <v>5.386765623108965</v>
+        <v>5.478868505840486</v>
       </c>
       <c r="C76">
-        <v>13.2272297658505</v>
+        <v>13.60795594704214</v>
       </c>
     </row>
     <row r="77">
@@ -1211,10 +1211,10 @@
         <v>24746</v>
       </c>
       <c r="B77">
-        <v>5.492593166478564</v>
+        <v>5.552983480717805</v>
       </c>
       <c r="C77">
-        <v>13.37605147744479</v>
+        <v>13.75234992559201</v>
       </c>
     </row>
     <row r="78">
@@ -1222,10 +1222,10 @@
         <v>24838</v>
       </c>
       <c r="B78">
-        <v>5.66501973035338</v>
+        <v>5.729158685522496</v>
       </c>
       <c r="C78">
-        <v>13.59338355592026</v>
+        <v>13.95980498043528</v>
       </c>
     </row>
     <row r="79">
@@ -1233,10 +1233,10 @@
         <v>24929</v>
       </c>
       <c r="B79">
-        <v>5.681509161855521</v>
+        <v>5.766771069940087</v>
       </c>
       <c r="C79">
-        <v>13.64404957108753</v>
+        <v>13.99467092922845</v>
       </c>
     </row>
     <row r="80">
@@ -1244,10 +1244,10 @@
         <v>25020</v>
       </c>
       <c r="B80">
-        <v>6.212445024981976</v>
+        <v>6.284368518733388</v>
       </c>
       <c r="C80">
-        <v>13.98507367700111</v>
+        <v>14.34477265859578</v>
       </c>
     </row>
     <row r="81">
@@ -1255,10 +1255,10 @@
         <v>25112</v>
       </c>
       <c r="B81">
-        <v>6.355833950303771</v>
+        <v>6.436059581384536</v>
       </c>
       <c r="C81">
-        <v>14.19085707077561</v>
+        <v>14.55876425730774</v>
       </c>
     </row>
     <row r="82">
@@ -1266,10 +1266,10 @@
         <v>25204</v>
       </c>
       <c r="B82">
-        <v>6.44747923805171</v>
+        <v>6.513084067719649</v>
       </c>
       <c r="C82">
-        <v>14.56050798512325</v>
+        <v>14.9258113897647</v>
       </c>
     </row>
     <row r="83">
@@ -1277,10 +1277,10 @@
         <v>25294</v>
       </c>
       <c r="B83">
-        <v>6.583276555270229</v>
+        <v>6.64660876881417</v>
       </c>
       <c r="C83">
-        <v>14.73249006891454</v>
+        <v>15.10550879842588</v>
       </c>
     </row>
     <row r="84">
@@ -1288,10 +1288,10 @@
         <v>25385</v>
       </c>
       <c r="B84">
-        <v>6.73631141531057</v>
+        <v>6.797969632574293</v>
       </c>
       <c r="C84">
-        <v>14.92140338605263</v>
+        <v>15.29604285616198</v>
       </c>
     </row>
     <row r="85">
@@ -1299,10 +1299,10 @@
         <v>25477</v>
       </c>
       <c r="B85">
-        <v>6.946074601726379</v>
+        <v>7.023729934189422</v>
       </c>
       <c r="C85">
-        <v>15.14901045020414</v>
+        <v>15.52767466953534</v>
       </c>
     </row>
     <row r="86">
@@ -1310,10 +1310,10 @@
         <v>25569</v>
       </c>
       <c r="B86">
-        <v>7.169001619705667</v>
+        <v>7.246937033633953</v>
       </c>
       <c r="C86">
-        <v>15.27253913580581</v>
+        <v>15.66423252798143</v>
       </c>
     </row>
     <row r="87">
@@ -1321,10 +1321,10 @@
         <v>25659</v>
       </c>
       <c r="B87">
-        <v>7.348796830624494</v>
+        <v>7.454080248967568</v>
       </c>
       <c r="C87">
-        <v>15.48810425214023</v>
+        <v>15.88198637031147</v>
       </c>
     </row>
     <row r="88">
@@ -1332,10 +1332,10 @@
         <v>25750</v>
       </c>
       <c r="B88">
-        <v>7.530582329473617</v>
+        <v>7.640643749417538</v>
       </c>
       <c r="C88">
-        <v>15.70222385283923</v>
+        <v>16.10287773432359</v>
       </c>
     </row>
     <row r="89">
@@ -1343,10 +1343,10 @@
         <v>25842</v>
       </c>
       <c r="B89">
-        <v>7.749818012545819</v>
+        <v>7.843262532450337</v>
       </c>
       <c r="C89">
-        <v>15.85345119532469</v>
+        <v>16.26132124384232</v>
       </c>
     </row>
     <row r="90">
@@ -1354,10 +1354,10 @@
         <v>25934</v>
       </c>
       <c r="B90">
-        <v>7.994880076155862</v>
+        <v>8.096451002097735</v>
       </c>
       <c r="C90">
-        <v>16.08833090952603</v>
+        <v>16.50807494766174</v>
       </c>
     </row>
     <row r="91">
@@ -1365,10 +1365,10 @@
         <v>26024</v>
       </c>
       <c r="B91">
-        <v>8.182512214360013</v>
+        <v>8.318875425559552</v>
       </c>
       <c r="C91">
-        <v>16.36425326283819</v>
+        <v>16.7824989891933</v>
       </c>
     </row>
     <row r="92">
@@ -1376,10 +1376,10 @@
         <v>26115</v>
       </c>
       <c r="B92">
-        <v>8.414451354192497</v>
+        <v>8.544687946427795</v>
       </c>
       <c r="C92">
-        <v>16.56082017630805</v>
+        <v>16.98454192780834</v>
       </c>
     </row>
     <row r="93">
@@ -1387,10 +1387,10 @@
         <v>26207</v>
       </c>
       <c r="B93">
-        <v>8.653062016075047</v>
+        <v>8.766128021190497</v>
       </c>
       <c r="C93">
-        <v>16.81356775921942</v>
+        <v>17.2306568077575</v>
       </c>
     </row>
     <row r="94">
@@ -1398,10 +1398,10 @@
         <v>26299</v>
       </c>
       <c r="B94">
-        <v>8.818316410513241</v>
+        <v>8.970395220329626</v>
       </c>
       <c r="C94">
-        <v>17.01065070885961</v>
+        <v>17.42054075495788</v>
       </c>
     </row>
     <row r="95">
@@ -1409,10 +1409,10 @@
         <v>26390</v>
       </c>
       <c r="B95">
-        <v>9.045638061353701</v>
+        <v>9.19305301809629</v>
       </c>
       <c r="C95">
-        <v>17.25689514938495</v>
+        <v>17.66418305455835</v>
       </c>
     </row>
     <row r="96">
@@ -1420,10 +1420,10 @@
         <v>26481</v>
       </c>
       <c r="B96">
-        <v>9.282918159061037</v>
+        <v>9.434269781566433</v>
       </c>
       <c r="C96">
-        <v>17.56441647101712</v>
+        <v>17.97589032627563</v>
       </c>
     </row>
     <row r="97">
@@ -1431,10 +1431,10 @@
         <v>26573</v>
       </c>
       <c r="B97">
-        <v>9.589189013209868</v>
+        <v>9.724649849421583</v>
       </c>
       <c r="C97">
-        <v>17.86349692495637</v>
+        <v>18.28899374832898</v>
       </c>
     </row>
     <row r="98">
@@ -1442,10 +1442,10 @@
         <v>26665</v>
       </c>
       <c r="B98">
-        <v>9.884268137281495</v>
+        <v>10.06021540115053</v>
       </c>
       <c r="C98">
-        <v>18.02626780600168</v>
+        <v>18.46587856845505</v>
       </c>
     </row>
     <row r="99">
@@ -1453,10 +1453,10 @@
         <v>26755</v>
       </c>
       <c r="B99">
-        <v>10.19446408791845</v>
+        <v>10.39266173882172</v>
       </c>
       <c r="C99">
-        <v>18.38435376659445</v>
+        <v>18.82953755766306</v>
       </c>
     </row>
     <row r="100">
@@ -1464,10 +1464,10 @@
         <v>26846</v>
       </c>
       <c r="B100">
-        <v>10.56660172148796</v>
+        <v>10.7525316032122</v>
       </c>
       <c r="C100">
-        <v>18.90107581841074</v>
+        <v>19.35171825141094</v>
       </c>
     </row>
     <row r="101">
@@ -1475,10 +1475,10 @@
         <v>26938</v>
       </c>
       <c r="B101">
-        <v>10.92923195285844</v>
+        <v>11.15734781712999</v>
       </c>
       <c r="C101">
-        <v>19.4386442520279</v>
+        <v>19.89538300893921</v>
       </c>
     </row>
     <row r="102">
@@ -1486,10 +1486,10 @@
         <v>27030</v>
       </c>
       <c r="B102">
-        <v>11.40870554987983</v>
+        <v>11.6017244165869</v>
       </c>
       <c r="C102">
-        <v>20.28138153470141</v>
+        <v>20.71050705241917</v>
       </c>
     </row>
     <row r="103">
@@ -1497,10 +1497,10 @@
         <v>27120</v>
       </c>
       <c r="B103">
-        <v>11.94411022935123</v>
+        <v>12.16026176260827</v>
       </c>
       <c r="C103">
-        <v>21.09532860594215</v>
+        <v>21.53120880220606</v>
       </c>
     </row>
     <row r="104">
@@ -1508,10 +1508,10 @@
         <v>27211</v>
       </c>
       <c r="B104">
-        <v>12.53639021089915</v>
+        <v>12.74849848421323</v>
       </c>
       <c r="C104">
-        <v>21.77831315241108</v>
+        <v>22.22032559689035</v>
       </c>
     </row>
     <row r="105">
@@ -1519,10 +1519,10 @@
         <v>27303</v>
       </c>
       <c r="B105">
-        <v>12.98755775747253</v>
+        <v>13.20973162330425</v>
       </c>
       <c r="C105">
-        <v>22.39797477436398</v>
+        <v>22.84725525119017</v>
       </c>
     </row>
     <row r="106">
@@ -1530,10 +1530,10 @@
         <v>27395</v>
       </c>
       <c r="B106">
-        <v>13.66199106665483</v>
+        <v>13.73097983700099</v>
       </c>
       <c r="C106">
-        <v>23.05334532262541</v>
+        <v>23.50457269937221</v>
       </c>
     </row>
     <row r="107">
@@ -1541,10 +1541,10 @@
         <v>27485</v>
       </c>
       <c r="B107">
-        <v>14.25519656124415</v>
+        <v>14.24912235798426</v>
       </c>
       <c r="C107">
-        <v>23.64716383456486</v>
+        <v>24.11219655520495</v>
       </c>
     </row>
     <row r="108">
@@ -1552,10 +1552,10 @@
         <v>27576</v>
       </c>
       <c r="B108">
-        <v>14.74039727508608</v>
+        <v>14.72377546561983</v>
       </c>
       <c r="C108">
-        <v>24.14456616677697</v>
+        <v>24.60990528213191</v>
       </c>
     </row>
     <row r="109">
@@ -1563,10 +1563,10 @@
         <v>27668</v>
       </c>
       <c r="B109">
-        <v>15.21636843856871</v>
+        <v>15.17319780298226</v>
       </c>
       <c r="C109">
-        <v>24.64524162921106</v>
+        <v>25.10292412294438</v>
       </c>
     </row>
     <row r="110">
@@ -1574,10 +1574,10 @@
         <v>27760</v>
       </c>
       <c r="B110">
-        <v>15.74579593409116</v>
+        <v>15.71242690424374</v>
       </c>
       <c r="C110">
-        <v>25.27707784632297</v>
+        <v>25.72515031513947</v>
       </c>
     </row>
     <row r="111">
@@ -1585,10 +1585,10 @@
         <v>27851</v>
       </c>
       <c r="B111">
-        <v>16.31076932014757</v>
+        <v>16.27664552708196</v>
       </c>
       <c r="C111">
-        <v>25.82895998058633</v>
+        <v>26.26960837908032</v>
       </c>
     </row>
     <row r="112">
@@ -1596,10 +1596,10 @@
         <v>27942</v>
       </c>
       <c r="B112">
-        <v>16.86175078595569</v>
+        <v>16.79807392830319</v>
       </c>
       <c r="C112">
-        <v>26.44508488596128</v>
+        <v>26.90655069254774</v>
       </c>
     </row>
     <row r="113">
@@ -1607,10 +1607,10 @@
         <v>28034</v>
       </c>
       <c r="B113">
-        <v>17.39334566001908</v>
+        <v>17.26481789094982</v>
       </c>
       <c r="C113">
-        <v>27.11806101313462</v>
+        <v>27.59100598499537</v>
       </c>
     </row>
     <row r="114">
@@ -1618,10 +1618,10 @@
         <v>28126</v>
       </c>
       <c r="B114">
-        <v>17.87217710419705</v>
+        <v>17.67007934940869</v>
       </c>
       <c r="C114">
-        <v>27.59683517367687</v>
+        <v>28.08157374804262</v>
       </c>
     </row>
     <row r="115">
@@ -1629,10 +1629,10 @@
         <v>28216</v>
       </c>
       <c r="B115">
-        <v>18.2674985914661</v>
+        <v>18.08133898591311</v>
       </c>
       <c r="C115">
-        <v>28.37714801064812</v>
+        <v>28.88927029639449</v>
       </c>
     </row>
     <row r="116">
@@ -1640,10 +1640,10 @@
         <v>28307</v>
       </c>
       <c r="B116">
-        <v>18.75562376312065</v>
+        <v>18.556174976673</v>
       </c>
       <c r="C116">
-        <v>28.99450413122559</v>
+        <v>29.51544606735928</v>
       </c>
     </row>
     <row r="117">
@@ -1651,10 +1651,10 @@
         <v>28399</v>
       </c>
       <c r="B117">
-        <v>19.31707850878407</v>
+        <v>19.12818125213544</v>
       </c>
       <c r="C117">
-        <v>29.48315171999855</v>
+        <v>30.01390807620106</v>
       </c>
     </row>
     <row r="118">
@@ -1662,10 +1662,10 @@
         <v>28491</v>
       </c>
       <c r="B118">
-        <v>19.83685818659943</v>
+        <v>19.69481900499757</v>
       </c>
       <c r="C118">
-        <v>29.92192993990717</v>
+        <v>30.46480605092577</v>
       </c>
     </row>
     <row r="119">
@@ -1673,10 +1673,10 @@
         <v>28581</v>
       </c>
       <c r="B119">
-        <v>20.42927431620927</v>
+        <v>20.28683376231011</v>
       </c>
       <c r="C119">
-        <v>30.65922622282446</v>
+        <v>31.2133998897043</v>
       </c>
     </row>
     <row r="120">
@@ -1684,10 +1684,10 @@
         <v>28672</v>
       </c>
       <c r="B120">
-        <v>21.06759569120547</v>
+        <v>20.89418427641475</v>
       </c>
       <c r="C120">
-        <v>31.53613180318635</v>
+        <v>32.08344559578651</v>
       </c>
     </row>
     <row r="121">
@@ -1695,10 +1695,10 @@
         <v>28764</v>
       </c>
       <c r="B121">
-        <v>21.66368344928861</v>
+        <v>21.44322970143001</v>
       </c>
       <c r="C121">
-        <v>32.27283364096644</v>
+        <v>32.84227835481595</v>
       </c>
     </row>
     <row r="122">
@@ -1706,10 +1706,10 @@
         <v>28856</v>
       </c>
       <c r="B122">
-        <v>22.27461276656224</v>
+        <v>21.9699525208727</v>
       </c>
       <c r="C122">
-        <v>33.01303709856683</v>
+        <v>33.5919120054634</v>
       </c>
     </row>
     <row r="123">
@@ -1717,10 +1717,10 @@
         <v>28946</v>
       </c>
       <c r="B123">
-        <v>23.03153768123375</v>
+        <v>22.56201404464463</v>
       </c>
       <c r="C123">
-        <v>33.91309449482218</v>
+        <v>34.49560823069081</v>
       </c>
     </row>
     <row r="124">
@@ -1728,10 +1728,10 @@
         <v>29037</v>
       </c>
       <c r="B124">
-        <v>23.78349368772271</v>
+        <v>23.28043287952672</v>
       </c>
       <c r="C124">
-        <v>35.08526235068669</v>
+        <v>35.6566956467869</v>
       </c>
     </row>
     <row r="125">
@@ -1739,10 +1739,10 @@
         <v>29129</v>
       </c>
       <c r="B125">
-        <v>24.64959534921233</v>
+        <v>24.16466262466599</v>
       </c>
       <c r="C125">
-        <v>35.9774917597757</v>
+        <v>36.55607090230576</v>
       </c>
     </row>
     <row r="126">
@@ -1750,10 +1750,10 @@
         <v>29221</v>
       </c>
       <c r="B126">
-        <v>25.47513062448815</v>
+        <v>25.04312418913895</v>
       </c>
       <c r="C126">
-        <v>37.32406866877337</v>
+        <v>37.75157457022692</v>
       </c>
     </row>
     <row r="127">
@@ -1761,10 +1761,10 @@
         <v>29312</v>
       </c>
       <c r="B127">
-        <v>26.42351320984924</v>
+        <v>26.00853451566119</v>
       </c>
       <c r="C127">
-        <v>38.42264568089002</v>
+        <v>39.09213117503321</v>
       </c>
     </row>
     <row r="128">
@@ -1772,10 +1772,10 @@
         <v>29403</v>
       </c>
       <c r="B128">
-        <v>27.30593697874337</v>
+        <v>26.89460571464578</v>
       </c>
       <c r="C128">
-        <v>39.569840711434</v>
+        <v>40.18311317574529</v>
       </c>
     </row>
     <row r="129">
@@ -1783,10 +1783,10 @@
         <v>29495</v>
       </c>
       <c r="B129">
-        <v>28.10851938451349</v>
+        <v>27.69308877265317</v>
       </c>
       <c r="C129">
-        <v>40.76430183627522</v>
+        <v>41.40157176052781</v>
       </c>
     </row>
     <row r="130">
@@ -1794,10 +1794,10 @@
         <v>29587</v>
       </c>
       <c r="B130">
-        <v>28.91467094497863</v>
+        <v>28.46790213806069</v>
       </c>
       <c r="C130">
-        <v>42.13520401748298</v>
+        <v>42.73894631249883</v>
       </c>
     </row>
     <row r="131">
@@ -1805,10 +1805,10 @@
         <v>29677</v>
       </c>
       <c r="B131">
-        <v>29.90874683657215</v>
+        <v>29.4447445128085</v>
       </c>
       <c r="C131">
-        <v>43.44769904633677</v>
+        <v>43.97767908165768</v>
       </c>
     </row>
     <row r="132">
@@ -1816,10 +1816,10 @@
         <v>29768</v>
       </c>
       <c r="B132">
-        <v>31.01600376567896</v>
+        <v>30.55834925010667</v>
       </c>
       <c r="C132">
-        <v>45.13858295982507</v>
+        <v>45.64923848286486</v>
       </c>
     </row>
     <row r="133">
@@ -1827,10 +1827,10 @@
         <v>29860</v>
       </c>
       <c r="B133">
-        <v>32.244893107301</v>
+        <v>31.77451418299099</v>
       </c>
       <c r="C133">
-        <v>46.56015578845248</v>
+        <v>47.16529116529007</v>
       </c>
     </row>
     <row r="134">
@@ -1838,10 +1838,10 @@
         <v>29952</v>
       </c>
       <c r="B134">
-        <v>33.58640738390994</v>
+        <v>32.95518465714238</v>
       </c>
       <c r="C134">
-        <v>47.88514129947569</v>
+        <v>48.49976718402314</v>
       </c>
     </row>
     <row r="135">
@@ -1849,10 +1849,10 @@
         <v>30042</v>
       </c>
       <c r="B135">
-        <v>34.46809357071259</v>
+        <v>33.82547571444941</v>
       </c>
       <c r="C135">
-        <v>49.22658811190679</v>
+        <v>49.78005421461752</v>
       </c>
     </row>
     <row r="136">
@@ -1860,10 +1860,10 @@
         <v>30133</v>
       </c>
       <c r="B136">
-        <v>35.06287441409685</v>
+        <v>34.29447970702632</v>
       </c>
       <c r="C136">
-        <v>50.02955304884757</v>
+        <v>50.63229140255087</v>
       </c>
     </row>
     <row r="137">
@@ -1871,10 +1871,10 @@
         <v>30225</v>
       </c>
       <c r="B137">
-        <v>35.7835509001213</v>
+        <v>34.90004621675762</v>
       </c>
       <c r="C137">
-        <v>51.04383519192312</v>
+        <v>51.57708990175208</v>
       </c>
     </row>
     <row r="138">
@@ -1882,10 +1882,10 @@
         <v>30317</v>
       </c>
       <c r="B138">
-        <v>36.8479153421768</v>
+        <v>35.80359727689172</v>
       </c>
       <c r="C138">
-        <v>52.39931855772426</v>
+        <v>52.97676529160741</v>
       </c>
     </row>
     <row r="139">
@@ -1893,10 +1893,10 @@
         <v>30407</v>
       </c>
       <c r="B139">
-        <v>37.59107680078307</v>
+        <v>36.57253888904153</v>
       </c>
       <c r="C139">
-        <v>53.77270391521779</v>
+        <v>54.44796233465439</v>
       </c>
     </row>
     <row r="140">
@@ -1904,10 +1904,10 @@
         <v>30498</v>
       </c>
       <c r="B140">
-        <v>38.57451818721826</v>
+        <v>37.28565089065813</v>
       </c>
       <c r="C140">
-        <v>54.95581949578163</v>
+        <v>55.56647192679046</v>
       </c>
     </row>
     <row r="141">
@@ -1915,10 +1915,10 @@
         <v>30590</v>
       </c>
       <c r="B141">
-        <v>39.42697627629011</v>
+        <v>38.02044821146891</v>
       </c>
       <c r="C141">
-        <v>56.08338814849182</v>
+        <v>56.68506866820312</v>
       </c>
     </row>
     <row r="142">
@@ -1926,10 +1926,10 @@
         <v>30682</v>
       </c>
       <c r="B142">
-        <v>40.20731836180652</v>
+        <v>38.76103742670002</v>
       </c>
       <c r="C142">
-        <v>57.14574465242721</v>
+        <v>57.79237088311501</v>
       </c>
     </row>
     <row r="143">
@@ -1937,10 +1937,10 @@
         <v>30773</v>
       </c>
       <c r="B143">
-        <v>41.13871877563336</v>
+        <v>39.45860783278123</v>
       </c>
       <c r="C143">
-        <v>58.07311274560944</v>
+        <v>58.73323908025828</v>
       </c>
     </row>
     <row r="144">
@@ -1948,10 +1948,10 @@
         <v>30864</v>
       </c>
       <c r="B144">
-        <v>41.39566941829618</v>
+        <v>40.07495577520011</v>
       </c>
       <c r="C144">
-        <v>59.08348416169177</v>
+        <v>59.68056571113225</v>
       </c>
     </row>
     <row r="145">
@@ -1959,10 +1959,10 @@
         <v>30956</v>
       </c>
       <c r="B145">
-        <v>42.34231025790423</v>
+        <v>40.66978229785275</v>
       </c>
       <c r="C145">
-        <v>60.07826459245612</v>
+        <v>60.74525545019561</v>
       </c>
     </row>
     <row r="146">
@@ -1970,10 +1970,10 @@
         <v>31048</v>
       </c>
       <c r="B146">
-        <v>43.10276707166051</v>
+        <v>41.32521645204889</v>
       </c>
       <c r="C146">
-        <v>61.02012703129161</v>
+        <v>61.80818564996904</v>
       </c>
     </row>
     <row r="147">
@@ -1981,10 +1981,10 @@
         <v>31138</v>
       </c>
       <c r="B147">
-        <v>43.7655500818136</v>
+        <v>41.90876382984107</v>
       </c>
       <c r="C147">
-        <v>62.03525712714041</v>
+        <v>62.61913731808407</v>
       </c>
     </row>
     <row r="148">
@@ -1992,10 +1992,10 @@
         <v>31229</v>
       </c>
       <c r="B148">
-        <v>44.28263335440145</v>
+        <v>42.48848652681873</v>
       </c>
       <c r="C148">
-        <v>62.66713656954676</v>
+        <v>63.34835662563604</v>
       </c>
     </row>
     <row r="149">
@@ -2003,10 +2003,10 @@
         <v>31321</v>
       </c>
       <c r="B149">
-        <v>44.81333771321702</v>
+        <v>43.08761979836914</v>
       </c>
       <c r="C149">
-        <v>63.14310369701091</v>
+        <v>63.84668797857703</v>
       </c>
     </row>
     <row r="150">
@@ -2014,10 +2014,10 @@
         <v>31413</v>
       </c>
       <c r="B150">
-        <v>45.1205786069892</v>
+        <v>43.570021175745</v>
       </c>
       <c r="C150">
-        <v>63.29432061285887</v>
+        <v>64.09036027568769</v>
       </c>
     </row>
     <row r="151">
@@ -2025,10 +2025,10 @@
         <v>31503</v>
       </c>
       <c r="B151">
-        <v>45.89273693345482</v>
+        <v>43.94796307283074</v>
       </c>
       <c r="C151">
-        <v>63.62354205399981</v>
+        <v>64.42523229967677</v>
       </c>
     </row>
     <row r="152">
@@ -2036,10 +2036,10 @@
         <v>31594</v>
       </c>
       <c r="B152">
-        <v>45.93520860048989</v>
+        <v>44.32719093968262</v>
       </c>
       <c r="C152">
-        <v>63.99025652723022</v>
+        <v>64.84006891596535</v>
       </c>
     </row>
     <row r="153">
@@ -2047,10 +2047,10 @@
         <v>31686</v>
       </c>
       <c r="B153">
-        <v>46.22605818792051</v>
+        <v>44.68859072279236</v>
       </c>
       <c r="C153">
-        <v>64.5854870104491</v>
+        <v>65.30161118366422</v>
       </c>
     </row>
     <row r="154">
@@ -2058,10 +2058,10 @@
         <v>31778</v>
       </c>
       <c r="B154">
-        <v>47.05877812724765</v>
+        <v>45.04505929554107</v>
       </c>
       <c r="C154">
-        <v>65.11371275396336</v>
+        <v>65.88350053403485</v>
       </c>
     </row>
     <row r="155">
@@ -2069,10 +2069,10 @@
         <v>31868</v>
       </c>
       <c r="B155">
-        <v>47.27809960021165</v>
+        <v>45.45302285970944</v>
       </c>
       <c r="C155">
-        <v>65.58660274857067</v>
+        <v>66.35360409813758</v>
       </c>
     </row>
     <row r="156">
@@ -2080,10 +2080,10 @@
         <v>31959</v>
       </c>
       <c r="B156">
-        <v>47.77090186224559</v>
+        <v>45.91420262443638</v>
       </c>
       <c r="C156">
-        <v>65.9858203736229</v>
+        <v>66.8423312261201</v>
       </c>
     </row>
     <row r="157">
@@ -2091,10 +2091,10 @@
         <v>32051</v>
       </c>
       <c r="B157">
-        <v>48.32549396248586</v>
+        <v>46.45203071441192</v>
       </c>
       <c r="C157">
-        <v>66.34137582326737</v>
+        <v>67.19295847855386</v>
       </c>
     </row>
     <row r="158">
@@ -2102,10 +2102,10 @@
         <v>32143</v>
       </c>
       <c r="B158">
-        <v>48.93704185562461</v>
+        <v>46.97838338296153</v>
       </c>
       <c r="C158">
-        <v>66.71107811955578</v>
+        <v>67.53394558940028</v>
       </c>
     </row>
     <row r="159">
@@ -2113,10 +2113,10 @@
         <v>32234</v>
       </c>
       <c r="B159">
-        <v>49.30435716885243</v>
+        <v>47.4707047610589</v>
       </c>
       <c r="C159">
-        <v>67.16234040802483</v>
+        <v>67.96294033706069</v>
       </c>
     </row>
     <row r="160">
@@ -2124,10 +2124,10 @@
         <v>32325</v>
       </c>
       <c r="B160">
-        <v>49.90225809816246</v>
+        <v>47.95283192140831</v>
       </c>
       <c r="C160">
-        <v>67.77502042001855</v>
+        <v>68.60539349591259</v>
       </c>
     </row>
     <row r="161">
@@ -2135,10 +2135,10 @@
         <v>32417</v>
       </c>
       <c r="B161">
-        <v>50.4369598161509</v>
+        <v>48.4318477075663</v>
       </c>
       <c r="C161">
-        <v>68.39824696205088</v>
+        <v>69.32631524301849</v>
       </c>
     </row>
     <row r="162">
@@ -2146,10 +2146,10 @@
         <v>32509</v>
       </c>
       <c r="B162">
-        <v>51.03045308549098</v>
+        <v>48.97795397394456</v>
       </c>
       <c r="C162">
-        <v>69.12224304254148</v>
+        <v>69.97660258902656</v>
       </c>
     </row>
     <row r="163">
@@ -2157,10 +2157,10 @@
         <v>32599</v>
       </c>
       <c r="B163">
-        <v>51.71162594080948</v>
+        <v>49.54974599785445</v>
       </c>
       <c r="C163">
-        <v>69.86967214598778</v>
+        <v>70.67493639792558</v>
       </c>
     </row>
     <row r="164">
@@ -2168,10 +2168,10 @@
         <v>32690</v>
       </c>
       <c r="B164">
-        <v>52.16954266095195</v>
+        <v>50.1145450451429</v>
       </c>
       <c r="C164">
-        <v>70.39250280940207</v>
+        <v>71.20652595172568</v>
       </c>
     </row>
     <row r="165">
@@ -2179,10 +2179,10 @@
         <v>32782</v>
       </c>
       <c r="B165">
-        <v>53.04683928735976</v>
+        <v>50.80465993634391</v>
       </c>
       <c r="C165">
-        <v>70.98444696242713</v>
+        <v>71.76483047997461</v>
       </c>
     </row>
     <row r="166">
@@ -2190,10 +2190,10 @@
         <v>32874</v>
       </c>
       <c r="B166">
-        <v>53.6921234630972</v>
+        <v>51.61372795941453</v>
       </c>
       <c r="C166">
-        <v>71.34622064292283</v>
+        <v>72.20164815006383</v>
       </c>
     </row>
     <row r="167">
@@ -2201,10 +2201,10 @@
         <v>32964</v>
       </c>
       <c r="B167">
-        <v>54.56319992823489</v>
+        <v>52.41445996437065</v>
       </c>
       <c r="C167">
-        <v>71.76936907401796</v>
+        <v>72.63217937851363</v>
       </c>
     </row>
     <row r="168">
@@ -2212,10 +2212,10 @@
         <v>33055</v>
       </c>
       <c r="B168">
-        <v>55.27845937956217</v>
+        <v>53.14042872561024</v>
       </c>
       <c r="C168">
-        <v>72.32597460577537</v>
+        <v>73.11516788177653</v>
       </c>
     </row>
     <row r="169">
@@ -2223,10 +2223,10 @@
         <v>33147</v>
       </c>
       <c r="B169">
-        <v>55.88491615424768</v>
+        <v>53.82506645637443</v>
       </c>
       <c r="C169">
-        <v>72.94526100706054</v>
+        <v>73.60172677499369</v>
       </c>
     </row>
     <row r="170">
@@ -2234,10 +2234,10 @@
         <v>33239</v>
       </c>
       <c r="B170">
-        <v>56.06469011261444</v>
+        <v>54.39551701859352</v>
       </c>
       <c r="C170">
-        <v>73.27880021079118</v>
+        <v>74.02256094255712</v>
       </c>
     </row>
     <row r="171">
@@ -2245,10 +2245,10 @@
         <v>33329</v>
       </c>
       <c r="B171">
-        <v>57.00185631813828</v>
+        <v>54.98316522588991</v>
       </c>
       <c r="C171">
-        <v>73.6639175662358</v>
+        <v>74.39884585657278</v>
       </c>
     </row>
     <row r="172">
@@ -2256,10 +2256,10 @@
         <v>33420</v>
       </c>
       <c r="B172">
-        <v>57.42081608848101</v>
+        <v>55.54360384780831</v>
       </c>
       <c r="C172">
-        <v>74.3045525422051</v>
+        <v>75.06206602746983</v>
       </c>
     </row>
     <row r="173">
@@ -2267,10 +2267,10 @@
         <v>33512</v>
       </c>
       <c r="B173">
-        <v>58.33194765456186</v>
+        <v>55.98899696733998</v>
       </c>
       <c r="C173">
-        <v>74.97218507941422</v>
+        <v>75.8152511550867</v>
       </c>
     </row>
     <row r="174">
@@ -2278,10 +2278,10 @@
         <v>33604</v>
       </c>
       <c r="B174">
-        <v>59.14173155134856</v>
+        <v>56.51871782251481</v>
       </c>
       <c r="C174">
-        <v>75.35460976625839</v>
+        <v>76.17484795646359</v>
       </c>
     </row>
     <row r="175">
@@ -2289,10 +2289,10 @@
         <v>33695</v>
       </c>
       <c r="B175">
-        <v>59.32241795315021</v>
+        <v>57.0614144324315</v>
       </c>
       <c r="C175">
-        <v>75.81443424397713</v>
+        <v>76.60831019506581</v>
       </c>
     </row>
     <row r="176">
@@ -2300,10 +2300,10 @@
         <v>33786</v>
       </c>
       <c r="B176">
-        <v>59.92873748171381</v>
+        <v>57.5078696312494</v>
       </c>
       <c r="C176">
-        <v>76.16158791379293</v>
+        <v>77.0068529604871</v>
       </c>
     </row>
     <row r="177">
@@ -2311,10 +2311,10 @@
         <v>33878</v>
       </c>
       <c r="B177">
-        <v>60.48989801961917</v>
+        <v>57.9296214550392</v>
       </c>
       <c r="C177">
-        <v>76.38433448680334</v>
+        <v>77.28152953055924</v>
       </c>
     </row>
     <row r="178">
@@ -2322,10 +2322,10 @@
         <v>33970</v>
       </c>
       <c r="B178">
-        <v>60.89416431466123</v>
+        <v>58.33164927325633</v>
       </c>
       <c r="C178">
-        <v>76.76736870055709</v>
+        <v>77.63182683303359</v>
       </c>
     </row>
     <row r="179">
@@ -2333,10 +2333,10 @@
         <v>34060</v>
       </c>
       <c r="B179">
-        <v>61.06094501528634</v>
+        <v>58.51050243142855</v>
       </c>
       <c r="C179">
-        <v>76.96097849409487</v>
+        <v>77.77448060804234</v>
       </c>
     </row>
     <row r="180">
@@ -2344,10 +2344,10 @@
         <v>34151</v>
       </c>
       <c r="B180">
-        <v>61.05736782992424</v>
+        <v>58.69873529166758</v>
       </c>
       <c r="C180">
-        <v>77.13566265778944</v>
+        <v>77.90468952429431</v>
       </c>
     </row>
     <row r="181">
@@ -2355,10 +2355,10 @@
         <v>34243</v>
       </c>
       <c r="B181">
-        <v>61.27087117449431</v>
+        <v>58.88615009197277</v>
       </c>
       <c r="C181">
-        <v>77.36840912604598</v>
+        <v>78.27074514267453</v>
       </c>
     </row>
     <row r="182">
@@ -2366,10 +2366,10 @@
         <v>34335</v>
       </c>
       <c r="B182">
-        <v>61.40594476550167</v>
+        <v>58.91195204147747</v>
       </c>
       <c r="C182">
-        <v>77.52894713900902</v>
+        <v>78.38598530054588</v>
       </c>
     </row>
     <row r="183">
@@ -2377,10 +2377,10 @@
         <v>34425</v>
       </c>
       <c r="B183">
-        <v>61.49298592718441</v>
+        <v>59.06569656030914</v>
       </c>
       <c r="C183">
-        <v>77.68469334311712</v>
+        <v>78.56098030771281</v>
       </c>
     </row>
     <row r="184">
@@ -2388,10 +2388,10 @@
         <v>34516</v>
       </c>
       <c r="B184">
-        <v>61.7832425543218</v>
+        <v>59.3800222091713</v>
       </c>
       <c r="C184">
-        <v>77.8552242036109</v>
+        <v>78.76362086243329</v>
       </c>
     </row>
     <row r="185">
@@ -2399,10 +2399,10 @@
         <v>34608</v>
       </c>
       <c r="B185">
-        <v>62.40401960382702</v>
+        <v>59.80183001276587</v>
       </c>
       <c r="C185">
-        <v>77.9619566229609</v>
+        <v>78.87316245657155</v>
       </c>
     </row>
     <row r="186">
@@ -2410,10 +2410,10 @@
         <v>34700</v>
       </c>
       <c r="B186">
-        <v>62.557340185875</v>
+        <v>60.27247817237858</v>
       </c>
       <c r="C186">
-        <v>78.1386672871464</v>
+        <v>79.07007279031235</v>
       </c>
     </row>
     <row r="187">
@@ -2421,10 +2421,10 @@
         <v>34790</v>
       </c>
       <c r="B187">
-        <v>62.97049114781765</v>
+        <v>60.71081741963535</v>
       </c>
       <c r="C187">
-        <v>78.18865018932436</v>
+        <v>79.15886365372116</v>
       </c>
     </row>
     <row r="188">
@@ -2432,10 +2432,10 @@
         <v>34881</v>
       </c>
       <c r="B188">
-        <v>63.13135103338902</v>
+        <v>61.05477802823843</v>
       </c>
       <c r="C188">
-        <v>78.59282147448329</v>
+        <v>79.50330207990547</v>
       </c>
     </row>
     <row r="189">
@@ -2443,10 +2443,10 @@
         <v>34973</v>
       </c>
       <c r="B189">
-        <v>63.23022086520162</v>
+        <v>61.33746754993945</v>
       </c>
       <c r="C189">
-        <v>78.93653848406356</v>
+        <v>79.83820834647476</v>
       </c>
     </row>
     <row r="190">
@@ -2454,10 +2454,10 @@
         <v>35065</v>
       </c>
       <c r="B190">
-        <v>63.64070196331011</v>
+        <v>61.63589954776708</v>
       </c>
       <c r="C190">
-        <v>79.41152648117928</v>
+        <v>80.29945865399517</v>
       </c>
     </row>
     <row r="191">
@@ -2465,10 +2465,10 @@
         <v>35156</v>
       </c>
       <c r="B191">
-        <v>64.02491259867533</v>
+        <v>61.95772640570251</v>
       </c>
       <c r="C191">
-        <v>79.7400855268869</v>
+        <v>80.60337044848436</v>
       </c>
     </row>
     <row r="192">
@@ -2476,10 +2476,10 @@
         <v>35247</v>
       </c>
       <c r="B192">
-        <v>64.32571149734902</v>
+        <v>62.21300890170036</v>
       </c>
       <c r="C192">
-        <v>79.63615672588575</v>
+        <v>80.51438915458549</v>
       </c>
     </row>
     <row r="193">
@@ -2487,10 +2487,10 @@
         <v>35339</v>
       </c>
       <c r="B193">
-        <v>64.34274216213333</v>
+        <v>62.44135151406002</v>
       </c>
       <c r="C193">
-        <v>79.93874828547052</v>
+        <v>80.82709003994057</v>
       </c>
     </row>
     <row r="194">
@@ -2498,10 +2498,10 @@
         <v>35431</v>
       </c>
       <c r="B194">
-        <v>64.70246514457264</v>
+        <v>62.6623858125465</v>
       </c>
       <c r="C194">
-        <v>80.19486413575584</v>
+        <v>81.06736805248455</v>
       </c>
     </row>
     <row r="195">
@@ -2509,10 +2509,10 @@
         <v>35521</v>
       </c>
       <c r="B195">
-        <v>64.96827269471819</v>
+        <v>62.93723778459304</v>
       </c>
       <c r="C195">
-        <v>80.09511977018468</v>
+        <v>80.97582238763643</v>
       </c>
     </row>
     <row r="196">
@@ -2520,10 +2520,10 @@
         <v>35612</v>
       </c>
       <c r="B196">
-        <v>65.22412903806631</v>
+        <v>63.31287975451758</v>
       </c>
       <c r="C196">
-        <v>80.3667458894832</v>
+        <v>81.27409569998289</v>
       </c>
     </row>
     <row r="197">
@@ -2531,10 +2531,10 @@
         <v>35704</v>
       </c>
       <c r="B197">
-        <v>65.32789264601671</v>
+        <v>63.65382062638457</v>
       </c>
       <c r="C197">
-        <v>80.58197809807127</v>
+        <v>81.41555264076791</v>
       </c>
     </row>
     <row r="198">
@@ -2542,10 +2542,10 @@
         <v>35796</v>
       </c>
       <c r="B198">
-        <v>65.75810348218468</v>
+        <v>63.95630076200356</v>
       </c>
       <c r="C198">
-        <v>80.63342808601507</v>
+        <v>81.4540866113625</v>
       </c>
     </row>
     <row r="199">
@@ -2553,10 +2553,10 @@
         <v>35886</v>
       </c>
       <c r="B199">
-        <v>65.93914632528988</v>
+        <v>64.25157167601108</v>
       </c>
       <c r="C199">
-        <v>80.66485224137753</v>
+        <v>81.45824470361134</v>
       </c>
     </row>
     <row r="200">
@@ -2564,10 +2564,10 @@
         <v>35977</v>
       </c>
       <c r="B200">
-        <v>66.43488153679168</v>
+        <v>64.74311278392459</v>
       </c>
       <c r="C200">
-        <v>80.45805192631228</v>
+        <v>81.2606399583253</v>
       </c>
     </row>
     <row r="201">
@@ -2575,10 +2575,10 @@
         <v>36069</v>
       </c>
       <c r="B201">
-        <v>66.66517864562557</v>
+        <v>65.01459500914017</v>
       </c>
       <c r="C201">
-        <v>80.09103113282801</v>
+        <v>81.01344312984914</v>
       </c>
     </row>
     <row r="202">
@@ -2586,10 +2586,10 @@
         <v>36161</v>
       </c>
       <c r="B202">
-        <v>66.97547543389301</v>
+        <v>65.10504480902331</v>
       </c>
       <c r="C202">
-        <v>79.92078411941101</v>
+        <v>80.77871771412434</v>
       </c>
     </row>
     <row r="203">
@@ -2597,10 +2597,10 @@
         <v>36251</v>
       </c>
       <c r="B203">
-        <v>67.08897025019613</v>
+        <v>65.50352481881212</v>
       </c>
       <c r="C203">
-        <v>79.93305806927702</v>
+        <v>80.80128965350455</v>
       </c>
     </row>
     <row r="204">
@@ -2608,10 +2608,10 @@
         <v>36342</v>
       </c>
       <c r="B204">
-        <v>67.47004451262026</v>
+        <v>65.89540183240648</v>
       </c>
       <c r="C204">
-        <v>79.86227170240045</v>
+        <v>80.76274606558981</v>
       </c>
     </row>
     <row r="205">
@@ -2619,10 +2619,10 @@
         <v>36434</v>
       </c>
       <c r="B205">
-        <v>68.02674430678253</v>
+        <v>66.51388111199589</v>
       </c>
       <c r="C205">
-        <v>80.32001259635884</v>
+        <v>81.22763629196128</v>
       </c>
     </row>
     <row r="206">
@@ -2630,10 +2630,10 @@
         <v>36526</v>
       </c>
       <c r="B206">
-        <v>68.6085394584528</v>
+        <v>67.32477662080414</v>
       </c>
       <c r="C206">
-        <v>81.0427707796006</v>
+        <v>81.80133634468103</v>
       </c>
     </row>
     <row r="207">
@@ -2641,10 +2641,10 @@
         <v>36617</v>
       </c>
       <c r="B207">
-        <v>68.82480111289449</v>
+        <v>67.8496597010012</v>
       </c>
       <c r="C207">
-        <v>81.47567620848545</v>
+        <v>82.2010107883945</v>
       </c>
     </row>
     <row r="208">
@@ -2652,10 +2652,10 @@
         <v>36708</v>
       </c>
       <c r="B208">
-        <v>69.26050859471812</v>
+        <v>68.30685907456684</v>
       </c>
       <c r="C208">
-        <v>82.14653580701759</v>
+        <v>82.8455088991127</v>
       </c>
     </row>
     <row r="209">
@@ -2663,10 +2663,10 @@
         <v>36800</v>
       </c>
       <c r="B209">
-        <v>70.03652358656495</v>
+        <v>69.2719502798878</v>
       </c>
       <c r="C209">
-        <v>82.77226565675878</v>
+        <v>83.47247904392242</v>
       </c>
     </row>
     <row r="210">
@@ -2674,10 +2674,10 @@
         <v>36892</v>
       </c>
       <c r="B210">
-        <v>70.05785170852774</v>
+        <v>69.80388503965911</v>
       </c>
       <c r="C210">
-        <v>82.87089179897801</v>
+        <v>83.48390299745947</v>
       </c>
     </row>
     <row r="211">
@@ -2685,10 +2685,10 @@
         <v>36982</v>
       </c>
       <c r="B211">
-        <v>70.74064999358595</v>
+        <v>69.92183992166932</v>
       </c>
       <c r="C211">
-        <v>83.55726237045222</v>
+        <v>84.15700960629576</v>
       </c>
     </row>
     <row r="212">
@@ -2696,10 +2696,10 @@
         <v>37073</v>
       </c>
       <c r="B212">
-        <v>71.15251539115334</v>
+        <v>70.44214453614048</v>
       </c>
       <c r="C212">
-        <v>83.70949269435798</v>
+        <v>84.29714949816098</v>
       </c>
     </row>
     <row r="213">
@@ -2707,10 +2707,10 @@
         <v>37165</v>
       </c>
       <c r="B213">
-        <v>71.68855744544736</v>
+        <v>70.98510839407346</v>
       </c>
       <c r="C213">
-        <v>83.65405239116212</v>
+        <v>84.21291403716793</v>
       </c>
     </row>
     <row r="214">
@@ -2718,10 +2718,10 @@
         <v>37257</v>
       </c>
       <c r="B214">
-        <v>72.22934786783</v>
+        <v>71.68736657672353</v>
       </c>
       <c r="C214">
-        <v>84.04735139235621</v>
+        <v>84.65962298681275</v>
       </c>
     </row>
     <row r="215">
@@ -2729,10 +2729,10 @@
         <v>37347</v>
       </c>
       <c r="B215">
-        <v>73.05114317193993</v>
+        <v>72.51758690236393</v>
       </c>
       <c r="C215">
-        <v>84.14813382472656</v>
+        <v>84.73790836200401</v>
       </c>
     </row>
     <row r="216">
@@ -2740,10 +2740,10 @@
         <v>37438</v>
       </c>
       <c r="B216">
-        <v>73.48030480241511</v>
+        <v>72.95698794912101</v>
       </c>
       <c r="C216">
-        <v>84.34795798807059</v>
+        <v>84.9027312248495</v>
       </c>
     </row>
     <row r="217">
@@ -2751,10 +2751,10 @@
         <v>37530</v>
       </c>
       <c r="B217">
-        <v>73.8552925013058</v>
+        <v>73.39767721355644</v>
       </c>
       <c r="C217">
-        <v>84.62431156248101</v>
+        <v>85.14524422104525</v>
       </c>
     </row>
     <row r="218">
@@ -2762,10 +2762,10 @@
         <v>37622</v>
       </c>
       <c r="B218">
-        <v>74.36784119249992</v>
+        <v>73.78303636211449</v>
       </c>
       <c r="C218">
-        <v>85.28809011080976</v>
+        <v>85.7842844377907</v>
       </c>
     </row>
     <row r="219">
@@ -2773,10 +2773,10 @@
         <v>37712</v>
       </c>
       <c r="B219">
-        <v>74.96661414048667</v>
+        <v>74.36510779928281</v>
       </c>
       <c r="C219">
-        <v>85.32241694738167</v>
+        <v>85.81395923994074</v>
       </c>
     </row>
     <row r="220">
@@ -2784,10 +2784,10 @@
         <v>37803</v>
       </c>
       <c r="B220">
-        <v>75.68424609696692</v>
+        <v>75.04565964916912</v>
       </c>
       <c r="C220">
-        <v>85.80114205998916</v>
+        <v>86.25267742022331</v>
       </c>
     </row>
     <row r="221">
@@ -2795,10 +2795,10 @@
         <v>37895</v>
       </c>
       <c r="B221">
-        <v>76.07047794390105</v>
+        <v>75.54495949877355</v>
       </c>
       <c r="C221">
-        <v>86.3294654194511</v>
+        <v>86.80003907262058</v>
       </c>
     </row>
     <row r="222">
@@ -2806,10 +2806,10 @@
         <v>37987</v>
       </c>
       <c r="B222">
-        <v>76.92794857991299</v>
+        <v>76.38825961801143</v>
       </c>
       <c r="C222">
-        <v>86.7500869761202</v>
+        <v>87.24370066120871</v>
       </c>
     </row>
     <row r="223">
@@ -2817,10 +2817,10 @@
         <v>38078</v>
       </c>
       <c r="B223">
-        <v>77.56506273935433</v>
+        <v>77.07451825992882</v>
       </c>
       <c r="C223">
-        <v>87.32519006741934</v>
+        <v>87.81940756288866</v>
       </c>
     </row>
     <row r="224">
@@ -2828,10 +2828,10 @@
         <v>38169</v>
       </c>
       <c r="B224">
-        <v>78.10725825480183</v>
+        <v>77.81558236741967</v>
       </c>
       <c r="C224">
-        <v>87.68999910757522</v>
+        <v>88.19638658971455</v>
       </c>
     </row>
     <row r="225">
@@ -2839,10 +2839,10 @@
         <v>38261</v>
       </c>
       <c r="B225">
-        <v>78.72158748630159</v>
+        <v>78.44893117536429</v>
       </c>
       <c r="C225">
-        <v>88.0723148360849</v>
+        <v>88.5554048066666</v>
       </c>
     </row>
     <row r="226">
@@ -2850,10 +2850,10 @@
         <v>38353</v>
       </c>
       <c r="B226">
-        <v>78.97461746803255</v>
+        <v>78.80948930438471</v>
       </c>
       <c r="C226">
-        <v>88.36340030360947</v>
+        <v>88.8297555871425</v>
       </c>
     </row>
     <row r="227">
@@ -2861,10 +2861,10 @@
         <v>38443</v>
       </c>
       <c r="B227">
-        <v>79.55115556607203</v>
+        <v>79.41704612499476</v>
       </c>
       <c r="C227">
-        <v>88.74998471982977</v>
+        <v>89.23468203822448</v>
       </c>
     </row>
     <row r="228">
@@ -2872,10 +2872,10 @@
         <v>38534</v>
       </c>
       <c r="B228">
-        <v>80.3172462644836</v>
+        <v>80.32803774241224</v>
       </c>
       <c r="C228">
-        <v>89.43039179318109</v>
+        <v>89.91837049863626</v>
       </c>
     </row>
     <row r="229">
@@ -2883,10 +2883,10 @@
         <v>38626</v>
       </c>
       <c r="B229">
-        <v>81.17822636029005</v>
+        <v>81.1471743118225</v>
       </c>
       <c r="C229">
-        <v>89.64123182354533</v>
+        <v>90.14753590833642</v>
       </c>
     </row>
     <row r="230">
@@ -2894,10 +2894,10 @@
         <v>38718</v>
       </c>
       <c r="B230">
-        <v>81.68847456825574</v>
+        <v>81.75719738035015</v>
       </c>
       <c r="C230">
-        <v>90.21109867339769</v>
+        <v>90.72276783994478</v>
       </c>
     </row>
     <row r="231">
@@ -2905,10 +2905,10 @@
         <v>38808</v>
       </c>
       <c r="B231">
-        <v>82.20345101875428</v>
+        <v>82.33626386554793</v>
       </c>
       <c r="C231">
-        <v>90.77693810106739</v>
+        <v>91.2971718827788</v>
       </c>
     </row>
     <row r="232">
@@ -2916,10 +2916,10 @@
         <v>38899</v>
       </c>
       <c r="B232">
-        <v>82.73747895794398</v>
+        <v>82.83277919349438</v>
       </c>
       <c r="C232">
-        <v>91.33582513416241</v>
+        <v>91.78884632550236</v>
       </c>
     </row>
     <row r="233">
@@ -2927,10 +2927,10 @@
         <v>38991</v>
       </c>
       <c r="B233">
-        <v>83.83362222750137</v>
+        <v>83.96480986049075</v>
       </c>
       <c r="C233">
-        <v>91.385083796586</v>
+        <v>91.7647213120661</v>
       </c>
     </row>
     <row r="234">
@@ -2938,10 +2938,10 @@
         <v>39083</v>
       </c>
       <c r="B234">
-        <v>84.05554142053978</v>
+        <v>84.31079067806412</v>
       </c>
       <c r="C234">
-        <v>91.77120767993301</v>
+        <v>92.08524882858531</v>
       </c>
     </row>
     <row r="235">
@@ -2949,10 +2949,10 @@
         <v>39173</v>
       </c>
       <c r="B235">
-        <v>84.31112162227548</v>
+        <v>84.68966180051251</v>
       </c>
       <c r="C235">
-        <v>92.44724951650544</v>
+        <v>92.71422903261988</v>
       </c>
     </row>
     <row r="236">
@@ -2960,10 +2960,10 @@
         <v>39264</v>
       </c>
       <c r="B236">
-        <v>84.73243731710983</v>
+        <v>85.22522999592351</v>
       </c>
       <c r="C236">
-        <v>93.11065019570255</v>
+        <v>93.34122819234611</v>
       </c>
     </row>
     <row r="237">
@@ -2971,10 +2971,10 @@
         <v>39356</v>
       </c>
       <c r="B237">
-        <v>85.51360619993726</v>
+        <v>85.87610481708587</v>
       </c>
       <c r="C237">
-        <v>94.10563356270202</v>
+        <v>94.33877821991797</v>
       </c>
     </row>
     <row r="238">
@@ -2982,10 +2982,10 @@
         <v>39448</v>
       </c>
       <c r="B238">
-        <v>86.32092164224055</v>
+        <v>86.79718124118122</v>
       </c>
       <c r="C238">
-        <v>95.01005446739214</v>
+        <v>95.3031087873245</v>
       </c>
     </row>
     <row r="239">
@@ -2993,10 +2993,10 @@
         <v>39539</v>
       </c>
       <c r="B239">
-        <v>86.50779096821758</v>
+        <v>87.04593532209292</v>
       </c>
       <c r="C239">
-        <v>95.91857334890183</v>
+        <v>96.23636544834972</v>
       </c>
     </row>
     <row r="240">
@@ -3004,10 +3004,10 @@
         <v>39630</v>
       </c>
       <c r="B240">
-        <v>87.09153219086672</v>
+        <v>87.59006648558064</v>
       </c>
       <c r="C240">
-        <v>95.90825520609003</v>
+        <v>96.22290737923524</v>
       </c>
     </row>
     <row r="241">
@@ -3015,10 +3015,10 @@
         <v>39722</v>
       </c>
       <c r="B241">
-        <v>86.98908827558827</v>
+        <v>87.57114286871297</v>
       </c>
       <c r="C241">
-        <v>94.97182322328237</v>
+        <v>95.29713623160026</v>
       </c>
     </row>
     <row r="242">
@@ -3026,10 +3026,10 @@
         <v>39814</v>
       </c>
       <c r="B242">
-        <v>87.11617305506985</v>
+        <v>87.59818509059815</v>
       </c>
       <c r="C242">
-        <v>94.2724739809278</v>
+        <v>94.55198635867063</v>
       </c>
     </row>
     <row r="243">
@@ -3037,10 +3037,10 @@
         <v>39904</v>
       </c>
       <c r="B243">
-        <v>87.34453333293945</v>
+        <v>87.7355767046229</v>
       </c>
       <c r="C243">
-        <v>93.8630100822831</v>
+        <v>94.09204877361903</v>
       </c>
     </row>
     <row r="244">
@@ -3048,10 +3048,10 @@
         <v>39995</v>
       </c>
       <c r="B244">
-        <v>87.95814500398764</v>
+        <v>88.37558269617767</v>
       </c>
       <c r="C244">
-        <v>93.78692842146252</v>
+        <v>94.00680642913434</v>
       </c>
     </row>
     <row r="245">
@@ -3059,10 +3059,10 @@
         <v>40087</v>
       </c>
       <c r="B245">
-        <v>88.67820972016162</v>
+        <v>89.04160556950559</v>
       </c>
       <c r="C245">
-        <v>93.88869719184616</v>
+        <v>94.1085212865036</v>
       </c>
     </row>
     <row r="246">
@@ -3070,10 +3070,10 @@
         <v>40179</v>
       </c>
       <c r="B246">
-        <v>89.54105867424326</v>
+        <v>90.10320737941058</v>
       </c>
       <c r="C246">
-        <v>94.47910215401004</v>
+        <v>94.73301633479436</v>
       </c>
     </row>
     <row r="247">
@@ -3081,10 +3081,10 @@
         <v>40269</v>
       </c>
       <c r="B247">
-        <v>90.20003328152984</v>
+        <v>90.83318862932805</v>
       </c>
       <c r="C247">
-        <v>94.99580118705565</v>
+        <v>95.2824240650223</v>
       </c>
     </row>
     <row r="248">
@@ -3092,10 +3092,10 @@
         <v>40360</v>
       </c>
       <c r="B248">
-        <v>90.52011307519844</v>
+        <v>91.15614668728327</v>
       </c>
       <c r="C248">
-        <v>95.18477440335397</v>
+        <v>95.49042727737822</v>
       </c>
     </row>
     <row r="249">
@@ -3103,10 +3103,10 @@
         <v>40452</v>
       </c>
       <c r="B249">
-        <v>90.76666039711061</v>
+        <v>91.41772538745816</v>
       </c>
       <c r="C249">
-        <v>95.51147028085587</v>
+        <v>95.81238010366364</v>
       </c>
     </row>
     <row r="250">
@@ -3114,10 +3114,10 @@
         <v>40544</v>
       </c>
       <c r="B250">
-        <v>91.41293024111388</v>
+        <v>91.85932935702012</v>
       </c>
       <c r="C250">
-        <v>96.22526200429733</v>
+        <v>96.52052334173159</v>
       </c>
     </row>
     <row r="251">
@@ -3125,10 +3125,10 @@
         <v>40634</v>
       </c>
       <c r="B251">
-        <v>91.51809684993415</v>
+        <v>91.75300089310321</v>
       </c>
       <c r="C251">
-        <v>96.69899348102768</v>
+        <v>96.97806220077031</v>
       </c>
     </row>
     <row r="252">
@@ -3136,10 +3136,10 @@
         <v>40725</v>
       </c>
       <c r="B252">
-        <v>91.59813196396489</v>
+        <v>91.80207086463457</v>
       </c>
       <c r="C252">
-        <v>96.92376750743826</v>
+        <v>97.17575065618861</v>
       </c>
     </row>
     <row r="253">
@@ -3147,10 +3147,10 @@
         <v>40817</v>
       </c>
       <c r="B253">
-        <v>92.19956626312225</v>
+        <v>92.20208527179072</v>
       </c>
       <c r="C253">
-        <v>97.30196037332557</v>
+        <v>97.54644505591298</v>
       </c>
     </row>
     <row r="254">
@@ -3158,10 +3158,10 @@
         <v>40909</v>
       </c>
       <c r="B254">
-        <v>92.63405376181585</v>
+        <v>92.71706599284272</v>
       </c>
       <c r="C254">
-        <v>97.92840589949982</v>
+        <v>98.14957590777843</v>
       </c>
     </row>
     <row r="255">
@@ -3169,10 +3169,10 @@
         <v>41000</v>
       </c>
       <c r="B255">
-        <v>92.88791007473431</v>
+        <v>92.8531275595974</v>
       </c>
       <c r="C255">
-        <v>98.1502497506134</v>
+        <v>98.35220159156528</v>
       </c>
     </row>
     <row r="256">
@@ -3180,10 +3180,10 @@
         <v>41091</v>
       </c>
       <c r="B256">
-        <v>93.28507278446978</v>
+        <v>93.31138163425958</v>
       </c>
       <c r="C256">
-        <v>98.18408287138631</v>
+        <v>98.34315107907258</v>
       </c>
     </row>
     <row r="257">
@@ -3191,10 +3191,10 @@
         <v>41183</v>
       </c>
       <c r="B257">
-        <v>93.7756516719792</v>
+        <v>93.60489281178094</v>
       </c>
       <c r="C257">
-        <v>98.32478292045798</v>
+        <v>98.45374958943216</v>
       </c>
     </row>
     <row r="258">
@@ -3202,10 +3202,10 @@
         <v>41275</v>
       </c>
       <c r="B258">
-        <v>93.79401521119287</v>
+        <v>93.76432035675501</v>
       </c>
       <c r="C258">
-        <v>98.70390590396265</v>
+        <v>98.83936067672536</v>
       </c>
     </row>
     <row r="259">
@@ -3213,10 +3213,10 @@
         <v>41365</v>
       </c>
       <c r="B259">
-        <v>94.36422182506342</v>
+        <v>94.27813359969773</v>
       </c>
       <c r="C259">
-        <v>98.68467557849651</v>
+        <v>98.8072090952181</v>
       </c>
     </row>
     <row r="260">
@@ -3224,10 +3224,10 @@
         <v>41456</v>
       </c>
       <c r="B260">
-        <v>94.83460759713613</v>
+        <v>94.5651944592276</v>
       </c>
       <c r="C260">
-        <v>98.88124558435372</v>
+        <v>99.00156148351425</v>
       </c>
     </row>
     <row r="261">
@@ -3235,10 +3235,10 @@
         <v>41548</v>
       </c>
       <c r="B261">
-        <v>94.84177192882588</v>
+        <v>94.62616140305968</v>
       </c>
       <c r="C261">
-        <v>98.85053612435574</v>
+        <v>98.97677241071902</v>
       </c>
     </row>
     <row r="262">
@@ -3246,10 +3246,10 @@
         <v>41640</v>
       </c>
       <c r="B262">
-        <v>95.1450408777077</v>
+        <v>94.64077741028774</v>
       </c>
       <c r="C262">
-        <v>99.06212530492053</v>
+        <v>99.18987164951967</v>
       </c>
     </row>
     <row r="263">
@@ -3257,10 +3257,10 @@
         <v>41730</v>
       </c>
       <c r="B263">
-        <v>95.4436451756894</v>
+        <v>94.84563304343966</v>
       </c>
       <c r="C263">
-        <v>98.88794518840032</v>
+        <v>99.03919492050865</v>
       </c>
     </row>
     <row r="264">
@@ -3268,10 +3268,10 @@
         <v>41821</v>
       </c>
       <c r="B264">
-        <v>95.78759029921345</v>
+        <v>95.13397786482032</v>
       </c>
       <c r="C264">
-        <v>98.79520288195174</v>
+        <v>98.95694300206571</v>
       </c>
     </row>
     <row r="265">
@@ -3279,10 +3279,10 @@
         <v>41913</v>
       </c>
       <c r="B265">
-        <v>96.06157591041169</v>
+        <v>95.2955542559619</v>
       </c>
       <c r="C265">
-        <v>98.7960468284631</v>
+        <v>98.92503197789138</v>
       </c>
     </row>
     <row r="266">
@@ -3290,10 +3290,10 @@
         <v>42005</v>
       </c>
       <c r="B266">
-        <v>96.29547973868512</v>
+        <v>95.80180976554006</v>
       </c>
       <c r="C266">
-        <v>98.81242469353822</v>
+        <v>98.9327261226836</v>
       </c>
     </row>
     <row r="267">
@@ -3301,10 +3301,10 @@
         <v>42095</v>
       </c>
       <c r="B267">
-        <v>96.71770320410995</v>
+        <v>96.30442753712261</v>
       </c>
       <c r="C267">
-        <v>99.29393136241579</v>
+        <v>99.40312609113194</v>
       </c>
     </row>
     <row r="268">
@@ -3312,10 +3312,10 @@
         <v>42186</v>
       </c>
       <c r="B268">
-        <v>97.10220429547637</v>
+        <v>96.62656421021369</v>
       </c>
       <c r="C268">
-        <v>99.24242561086196</v>
+        <v>99.35651451174373</v>
       </c>
     </row>
     <row r="269">
@@ -3323,10 +3323,10 @@
         <v>42278</v>
       </c>
       <c r="B269">
-        <v>97.58651595042708</v>
+        <v>97.2180985647052</v>
       </c>
       <c r="C269">
-        <v>99.22724347971629</v>
+        <v>99.31843090818956</v>
       </c>
     </row>
     <row r="270">
@@ -3334,10 +3334,10 @@
         <v>42370</v>
       </c>
       <c r="B270">
-        <v>98.17429380511271</v>
+        <v>97.70389856287312</v>
       </c>
       <c r="C270">
-        <v>99.06839119939586</v>
+        <v>99.14012820042416</v>
       </c>
     </row>
     <row r="271">
@@ -3345,10 +3345,10 @@
         <v>42461</v>
       </c>
       <c r="B271">
-        <v>98.04573787064433</v>
+        <v>97.86590229301098</v>
       </c>
       <c r="C271">
-        <v>99.34220506187171</v>
+        <v>99.42389367775994</v>
       </c>
     </row>
     <row r="272">
@@ -3356,10 +3356,10 @@
         <v>42552</v>
       </c>
       <c r="B272">
-        <v>98.35996862786484</v>
+        <v>98.27737404608902</v>
       </c>
       <c r="C272">
-        <v>99.42646655590795</v>
+        <v>99.51263554204766</v>
       </c>
     </row>
     <row r="273">
@@ -3367,10 +3367,10 @@
         <v>42644</v>
       </c>
       <c r="B273">
-        <v>98.91113723459651</v>
+        <v>98.75468334000907</v>
       </c>
       <c r="C273">
-        <v>99.63600387854346</v>
+        <v>99.71346757569997</v>
       </c>
     </row>
     <row r="274">
@@ -3378,10 +3378,10 @@
         <v>42736</v>
       </c>
       <c r="B274">
-        <v>99.79714644362268</v>
+        <v>99.67805795437138</v>
       </c>
       <c r="C274">
-        <v>100.0524603942098</v>
+        <v>100.0092838483505</v>
       </c>
     </row>
     <row r="275">
@@ -3400,10 +3400,10 @@
         <v>42917</v>
       </c>
       <c r="B276">
-        <v>100.3615738671262</v>
+        <v>100.3198190095528</v>
       </c>
       <c r="C276">
-        <v>100.0439751843059</v>
+        <v>100.1278091292464</v>
       </c>
     </row>
     <row r="277">
@@ -3411,10 +3411,10 @@
         <v>43009</v>
       </c>
       <c r="B277">
-        <v>101.195241366691</v>
+        <v>100.7168015887696</v>
       </c>
       <c r="C277">
-        <v>100.5905809971437</v>
+        <v>100.7168626259664</v>
       </c>
     </row>
     <row r="278">
@@ -3422,10 +3422,10 @@
         <v>43101</v>
       </c>
       <c r="B278">
-        <v>101.2087168529435</v>
+        <v>100.7786235490665</v>
       </c>
       <c r="C278">
-        <v>101.2674450582879</v>
+        <v>101.4571326781975</v>
       </c>
     </row>
     <row r="279">
@@ -3433,10 +3433,10 @@
         <v>43191</v>
       </c>
       <c r="B279">
-        <v>101.7162582497874</v>
+        <v>101.4366434011637</v>
       </c>
       <c r="C279">
-        <v>101.8433383184556</v>
+        <v>102.1496062578734</v>
       </c>
     </row>
     <row r="280">
@@ -3444,10 +3444,10 @@
         <v>43282</v>
       </c>
       <c r="B280">
-        <v>102.3257475915487</v>
+        <v>101.9978594942991</v>
       </c>
       <c r="C280">
-        <v>102.119486592023</v>
+        <v>102.4486280053882</v>
       </c>
     </row>
     <row r="281">
@@ -3455,10 +3455,10 @@
         <v>43374</v>
       </c>
       <c r="B281">
-        <v>102.8432591869217</v>
+        <v>102.6958733233645</v>
       </c>
       <c r="C281">
-        <v>102.2287339862874</v>
+        <v>102.5290498488953</v>
       </c>
     </row>
     <row r="282">
@@ -3466,10 +3466,10 @@
         <v>43466</v>
       </c>
       <c r="B282">
-        <v>101.4742354335517</v>
+        <v>103.7694816063694</v>
       </c>
       <c r="C282">
-        <v>102.2237701537</v>
+        <v>102.4817455442761</v>
       </c>
     </row>
     <row r="283">
@@ -3477,10 +3477,10 @@
         <v>43556</v>
       </c>
       <c r="B283">
-        <v>101.1043185977434</v>
+        <v>103.6236726211591</v>
       </c>
       <c r="C283">
-        <v>102.5960904164361</v>
+        <v>102.8523517018521</v>
       </c>
     </row>
     <row r="284">
@@ -3488,10 +3488,10 @@
         <v>43647</v>
       </c>
       <c r="B284">
-        <v>101.3074314814449</v>
+        <v>104.2731180631373</v>
       </c>
       <c r="C284">
-        <v>102.822015215222</v>
+        <v>103.0728624711082</v>
       </c>
     </row>
     <row r="285">
@@ -3499,10 +3499,10 @@
         <v>43739</v>
       </c>
       <c r="B285">
-        <v>101.0307787680512</v>
+        <v>104.0280803337737</v>
       </c>
       <c r="C285">
-        <v>103.1846460591515</v>
+        <v>103.4120264330004</v>
       </c>
     </row>
     <row r="286">
@@ -3510,10 +3510,10 @@
         <v>43831</v>
       </c>
       <c r="B286">
-        <v>97.33284694670377</v>
+        <v>100.2409270587852</v>
       </c>
       <c r="C286">
-        <v>103.5174823801417</v>
+        <v>103.6407511756955</v>
       </c>
     </row>
     <row r="287">
@@ -3521,10 +3521,10 @@
         <v>43922</v>
       </c>
       <c r="B287">
-        <v>85.96181432337926</v>
+        <v>88.41511079436432</v>
       </c>
       <c r="C287">
-        <v>103.5944757923636</v>
+        <v>103.6495051473229</v>
       </c>
     </row>
     <row r="288">
@@ -3532,10 +3532,10 @@
         <v>44013</v>
       </c>
       <c r="B288">
-        <v>99.19393515917464</v>
+        <v>101.842257148184</v>
       </c>
       <c r="C288">
-        <v>103.6081143644015</v>
+        <v>103.754674922693</v>
       </c>
     </row>
     <row r="289">
@@ -3543,10 +3543,10 @@
         <v>44105</v>
       </c>
       <c r="B289">
-        <v>97.56972434121603</v>
+        <v>100.1814456696542</v>
       </c>
       <c r="C289">
-        <v>103.7404082041653</v>
+        <v>103.8593830039399</v>
       </c>
     </row>
     <row r="290">
@@ -3554,10 +3554,10 @@
         <v>44197</v>
       </c>
       <c r="B290">
-        <v>97.70807666653921</v>
+        <v>100.2401500152731</v>
       </c>
       <c r="C290">
-        <v>104.3511384616094</v>
+        <v>104.3842345327405</v>
       </c>
     </row>
     <row r="291">
@@ -3565,10 +3565,10 @@
         <v>44287</v>
       </c>
       <c r="B291">
-        <v>98.78568676741693</v>
+        <v>101.5986202574854</v>
       </c>
       <c r="C291">
-        <v>104.6558823369027</v>
+        <v>104.6961021867737</v>
       </c>
     </row>
     <row r="292">
@@ -3576,10 +3576,10 @@
         <v>44378</v>
       </c>
       <c r="B292">
-        <v>101.8150422111389</v>
+        <v>105.1092662976429</v>
       </c>
       <c r="C292">
-        <v>105.3801306291325</v>
+        <v>105.3759555452453</v>
       </c>
     </row>
     <row r="293">
@@ -3587,10 +3587,10 @@
         <v>44470</v>
       </c>
       <c r="B293">
-        <v>102.4245916124575</v>
+        <v>105.921905766465</v>
       </c>
       <c r="C293">
-        <v>106.2061457923502</v>
+        <v>106.0164833539689</v>
       </c>
     </row>
     <row r="294">
@@ -3598,10 +3598,10 @@
         <v>44562</v>
       </c>
       <c r="B294">
-        <v>103.8027925876426</v>
+        <v>106.8651199595839</v>
       </c>
       <c r="C294">
-        <v>107.3509503836638</v>
+        <v>107.2605858052747</v>
       </c>
     </row>
     <row r="295">
@@ -3609,10 +3609,10 @@
         <v>44652</v>
       </c>
       <c r="B295">
-        <v>104.5078433050086</v>
+        <v>107.8543002311287</v>
       </c>
       <c r="C295">
-        <v>109.2877821642938</v>
+        <v>109.2200468987831</v>
       </c>
     </row>
     <row r="296">
@@ -3620,10 +3620,10 @@
         <v>44743</v>
       </c>
       <c r="B296">
-        <v>104.6527936254914</v>
+        <v>109.0508348452472</v>
       </c>
       <c r="C296">
-        <v>111.1118798993653</v>
+        <v>111.1589337341948</v>
       </c>
     </row>
     <row r="297">
@@ -3631,10 +3631,10 @@
         <v>44835</v>
       </c>
       <c r="B297">
-        <v>106.7790050297514</v>
+        <v>110.7718734922877</v>
       </c>
       <c r="C297">
-        <v>113.2787923525218</v>
+        <v>113.5070710599694</v>
       </c>
     </row>
     <row r="298">
@@ -3642,18 +3642,62 @@
         <v>44927</v>
       </c>
       <c r="B298">
-        <v>107.9790291168578</v>
+        <v>111.8088217832836</v>
       </c>
       <c r="C298">
-        <v>115.5941037192763</v>
+        <v>116.0224345240727</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="2">
         <v>45017</v>
       </c>
+      <c r="B299">
+        <v>112.6293836347398</v>
+      </c>
       <c r="C299">
-        <v>117.0290906371843</v>
+        <v>117.825236388378</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="2">
+        <v>45108</v>
+      </c>
+      <c r="B300">
+        <v>113.0872632485201</v>
+      </c>
+      <c r="C300">
+        <v>119.0926692449106</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="2">
+        <v>45200</v>
+      </c>
+      <c r="B301">
+        <v>114.0464513586812</v>
+      </c>
+      <c r="C301">
+        <v>119.4640101899286</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="2">
+        <v>45292</v>
+      </c>
+      <c r="B302">
+        <v>115.0944059851962</v>
+      </c>
+      <c r="C302">
+        <v>120.2807595657745</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="2">
+        <v>45383</v>
+      </c>
+      <c r="C303">
+        <v>120.7377624437748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>